<commit_message>
update usage-company.xlsx 2025-10-02 17:09:47
</commit_message>
<xml_diff>
--- a/usage-company.xlsx
+++ b/usage-company.xlsx
@@ -9885,7 +9885,7 @@
         <v>23253</v>
       </c>
       <c r="M141" t="n">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="N141" t="n">
         <v>0</v>
@@ -9894,7 +9894,7 @@
         <v>0</v>
       </c>
       <c r="P141" t="n">
-        <v>78813</v>
+        <v>78815</v>
       </c>
       <c r="Q141" t="inlineStr">
         <is>
@@ -35433,10 +35433,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S522" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S522" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="523">
@@ -35502,10 +35500,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S523" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S523" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="524">
@@ -35571,10 +35567,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S524" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S524" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="525">
@@ -35640,10 +35634,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S525" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S525" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="526">
@@ -35709,10 +35701,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S526" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S526" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="527">
@@ -35778,10 +35768,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S527" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S527" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="528">
@@ -35847,10 +35835,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S528" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S528" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="529">
@@ -35916,10 +35902,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S529" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S529" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="530">
@@ -35985,10 +35969,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S530" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S530" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="531">
@@ -36054,10 +36036,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S531" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S531" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="532">
@@ -36123,10 +36103,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S532" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S532" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="533">
@@ -36192,10 +36170,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S533" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S533" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="534">
@@ -36261,10 +36237,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S534" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S534" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="535">
@@ -36330,10 +36304,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S535" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S535" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="536">
@@ -36399,10 +36371,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S536" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S536" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="537">
@@ -36468,10 +36438,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S537" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S537" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="538">
@@ -36537,10 +36505,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S538" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S538" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="539">
@@ -36606,10 +36572,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S539" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S539" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="540">
@@ -36675,10 +36639,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S540" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S540" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="541">
@@ -36744,10 +36706,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S541" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S541" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="542">
@@ -36813,10 +36773,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S542" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S542" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="543">
@@ -36882,10 +36840,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S543" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S543" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="544">
@@ -36951,10 +36907,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S544" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S544" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="545">
@@ -37020,10 +36974,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S545" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S545" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="546">
@@ -37089,10 +37041,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S546" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S546" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="547">
@@ -37158,10 +37108,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S547" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S547" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="548">
@@ -37227,10 +37175,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S548" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S548" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="549">
@@ -37296,10 +37242,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S549" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S549" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="550">
@@ -37365,10 +37309,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S550" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S550" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="551">
@@ -37434,10 +37376,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S551" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S551" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="552">
@@ -37503,10 +37443,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S552" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S552" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="553">
@@ -37572,10 +37510,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S553" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S553" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="554">
@@ -37641,10 +37577,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S554" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S554" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="555">
@@ -37710,10 +37644,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S555" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S555" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="556">
@@ -37779,10 +37711,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S556" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S556" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="557">
@@ -37848,10 +37778,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S557" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S557" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="558">
@@ -37917,10 +37845,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S558" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S558" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="559">
@@ -37986,10 +37912,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S559" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S559" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="560">
@@ -38055,10 +37979,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S560" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S560" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="561">
@@ -38124,10 +38046,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S561" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S561" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="562">
@@ -38193,10 +38113,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S562" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S562" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="563">
@@ -38262,10 +38180,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S563" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S563" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="564">
@@ -38331,10 +38247,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S564" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S564" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="565">
@@ -38400,10 +38314,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S565" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S565" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="566">
@@ -38469,10 +38381,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S566" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S566" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="567">
@@ -38538,10 +38448,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S567" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S567" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="568">
@@ -38607,10 +38515,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S568" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S568" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="569">
@@ -38676,10 +38582,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S569" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S569" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="570">
@@ -38745,10 +38649,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S570" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S570" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="571">
@@ -38814,10 +38716,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S571" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S571" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="572">
@@ -38883,10 +38783,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S572" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S572" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="573">
@@ -38952,10 +38850,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S573" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S573" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="574">
@@ -39021,10 +38917,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S574" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S574" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="575">
@@ -39090,10 +38984,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S575" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S575" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="576">
@@ -39159,10 +39051,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S576" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S576" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="577">
@@ -39228,10 +39118,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S577" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S577" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="578">
@@ -39297,10 +39185,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S578" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S578" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="579">
@@ -39366,10 +39252,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S579" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S579" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="580">
@@ -39435,10 +39319,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S580" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S580" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="581">
@@ -39504,10 +39386,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S581" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S581" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="582">
@@ -39573,10 +39453,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S582" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S582" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="583">
@@ -39642,10 +39520,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S583" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S583" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="584">
@@ -39711,10 +39587,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S584" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S584" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="585">
@@ -39780,10 +39654,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S585" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S585" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="586">
@@ -39849,10 +39721,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S586" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S586" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="587">
@@ -39918,10 +39788,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S587" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S587" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="588">
@@ -39987,10 +39855,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S588" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S588" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="589">
@@ -40056,10 +39922,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S589" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S589" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="590">
@@ -40125,10 +39989,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S590" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S590" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="591">
@@ -40194,10 +40056,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S591" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S591" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="592">
@@ -40263,10 +40123,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S592" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S592" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="593">
@@ -40332,10 +40190,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S593" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S593" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="594">
@@ -40401,10 +40257,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S594" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S594" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="595">
@@ -40470,10 +40324,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S595" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S595" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="596">
@@ -40539,10 +40391,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S596" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S596" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="597">
@@ -40608,10 +40458,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S597" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S597" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="598">
@@ -40677,10 +40525,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S598" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S598" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="599">
@@ -40746,10 +40592,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S599" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S599" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="600">
@@ -40815,10 +40659,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S600" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S600" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="601">
@@ -40884,10 +40726,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S601" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S601" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="602">
@@ -40953,10 +40793,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S602" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S602" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="603">
@@ -41022,10 +40860,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S603" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S603" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="604">
@@ -41091,10 +40927,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S604" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S604" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="605">
@@ -41160,10 +40994,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S605" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S605" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="606">
@@ -41229,10 +41061,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S606" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S606" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="607">
@@ -41298,10 +41128,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S607" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S607" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="608">
@@ -41367,10 +41195,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S608" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S608" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="609">
@@ -41436,10 +41262,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S609" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S609" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="610">
@@ -41505,10 +41329,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S610" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S610" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="611">
@@ -41574,10 +41396,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S611" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S611" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="612">
@@ -41643,10 +41463,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S612" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S612" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="613">
@@ -41712,10 +41530,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S613" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S613" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="614">
@@ -41781,10 +41597,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S614" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S614" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="615">
@@ -41850,10 +41664,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S615" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S615" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="616">
@@ -41919,10 +41731,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S616" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S616" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="617">
@@ -41988,10 +41798,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S617" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S617" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="618">
@@ -42057,10 +41865,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S618" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S618" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="619">
@@ -42126,10 +41932,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S619" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S619" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="620">
@@ -42195,10 +41999,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S620" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S620" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="621">
@@ -42264,10 +42066,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S621" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S621" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="622">
@@ -42333,10 +42133,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S622" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S622" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="623">
@@ -42402,10 +42200,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S623" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S623" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="624">
@@ -42471,10 +42267,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S624" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S624" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="625">
@@ -42540,10 +42334,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S625" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S625" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="626">
@@ -42609,10 +42401,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S626" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S626" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="627">
@@ -42678,10 +42468,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S627" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S627" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="628">
@@ -42747,10 +42535,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S628" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S628" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="629">
@@ -42816,10 +42602,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S629" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S629" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="630">
@@ -42885,10 +42669,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S630" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S630" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="631">
@@ -42954,10 +42736,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S631" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S631" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="632">
@@ -43023,10 +42803,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S632" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S632" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="633">
@@ -43092,10 +42870,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S633" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S633" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="634">
@@ -43161,10 +42937,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S634" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S634" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="635">
@@ -43230,10 +43004,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S635" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S635" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="636">
@@ -43299,10 +43071,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S636" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S636" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="637">
@@ -43368,10 +43138,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S637" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S637" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="638">
@@ -43437,10 +43205,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S638" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S638" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="639">
@@ -43506,10 +43272,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S639" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S639" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="640">
@@ -43575,10 +43339,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S640" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S640" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="641">
@@ -43644,10 +43406,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S641" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S641" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="642">
@@ -43713,10 +43473,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S642" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S642" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="643">
@@ -43782,10 +43540,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S643" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S643" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="644">
@@ -43851,10 +43607,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S644" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S644" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="645">
@@ -43920,10 +43674,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S645" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S645" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="646">
@@ -43989,10 +43741,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S646" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S646" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="647">
@@ -44058,10 +43808,8 @@
           <t>dalam-negri</t>
         </is>
       </c>
-      <c r="S647" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S647" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="648">
@@ -44127,10 +43875,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S648" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S648" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="649">
@@ -44196,10 +43942,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S649" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S649" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="650">
@@ -44265,10 +44009,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S650" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S650" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="651">
@@ -44334,10 +44076,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S651" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S651" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="652">
@@ -44403,10 +44143,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S652" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S652" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="653">
@@ -44472,10 +44210,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S653" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S653" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="654">
@@ -44541,10 +44277,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S654" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S654" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="655">
@@ -44610,10 +44344,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S655" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S655" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="656">
@@ -44679,10 +44411,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S656" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S656" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="657">
@@ -44748,10 +44478,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S657" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S657" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="658">
@@ -44817,10 +44545,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S658" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S658" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="659">
@@ -44886,10 +44612,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S659" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S659" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="660">
@@ -44955,10 +44679,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S660" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S660" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="661">
@@ -45024,10 +44746,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S661" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S661" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="662">
@@ -45093,10 +44813,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S662" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S662" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="663">
@@ -45162,10 +44880,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S663" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S663" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="664">
@@ -45231,10 +44947,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S664" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S664" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="665">
@@ -45300,10 +45014,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S665" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S665" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="666">
@@ -45369,10 +45081,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S666" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S666" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="667">
@@ -45438,10 +45148,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S667" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S667" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="668">
@@ -45507,10 +45215,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S668" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S668" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="669">
@@ -45576,10 +45282,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S669" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S669" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="670">
@@ -45645,10 +45349,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S670" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S670" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="671">
@@ -45714,10 +45416,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S671" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S671" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="672">
@@ -45783,10 +45483,8 @@
           <t>luar-negri</t>
         </is>
       </c>
-      <c r="S672" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S672" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="673">
@@ -45852,10 +45550,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S673" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S673" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="674">
@@ -45921,10 +45617,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S674" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S674" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="675">
@@ -45990,10 +45684,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S675" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S675" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="676">
@@ -46059,10 +45751,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S676" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S676" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="677">
@@ -46128,10 +45818,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S677" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S677" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="678">
@@ -46197,10 +45885,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S678" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S678" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="679">
@@ -46266,10 +45952,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S679" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S679" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="680">
@@ -46335,10 +46019,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S680" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S680" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="681">
@@ -46404,10 +46086,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S681" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S681" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="682">
@@ -46473,10 +46153,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S682" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S682" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="683">
@@ -46542,10 +46220,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S683" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S683" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="684">
@@ -46611,10 +46287,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S684" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S684" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="685">
@@ -46680,10 +46354,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S685" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S685" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="686">
@@ -46749,10 +46421,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S686" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S686" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="687">
@@ -46818,10 +46488,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S687" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S687" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="688">
@@ -46887,10 +46555,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S688" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S688" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="689">
@@ -46956,10 +46622,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S689" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S689" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="690">
@@ -47025,10 +46689,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S690" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S690" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="691">
@@ -47094,10 +46756,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S691" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S691" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="692">
@@ -47163,10 +46823,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S692" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S692" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="693">
@@ -47232,10 +46890,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S693" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S693" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="694">
@@ -47301,10 +46957,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S694" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S694" t="n">
+        <v>2025</v>
       </c>
     </row>
     <row r="695">
@@ -47370,10 +47024,8 @@
           <t>self</t>
         </is>
       </c>
-      <c r="S695" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="S695" t="n">
+        <v>2025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>